<commit_message>
updated PSI test results
</commit_message>
<xml_diff>
--- a/waferstatus_20150925.xlsx
+++ b/waferstatus_20150925.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="376">
   <si>
     <t>Wafer</t>
   </si>
@@ -1150,10 +1150,28 @@
     <t>4QJZB00000</t>
   </si>
   <si>
-    <t>4QJZB00020</t>
-  </si>
-  <si>
     <t>#potential BM</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>V56CDVX</t>
+  </si>
+  <si>
+    <t>VA6CC8X</t>
+  </si>
+  <si>
+    <t>V86CDSX</t>
+  </si>
+  <si>
+    <t>VF6CDKX</t>
+  </si>
+  <si>
+    <t>4KSGB00B30</t>
   </si>
 </sst>
 </file>
@@ -1505,7 +1523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1885,13 +1903,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1899,6 +1923,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1927,19 +1954,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2246,13 +2270,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:U200"/>
+  <dimension ref="B1:U204"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="F129" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F135" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P162" sqref="P162"/>
+      <selection pane="bottomRight" activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2278,20 +2302,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="D1" s="158" t="s">
+      <c r="D1" s="161" t="s">
         <v>277</v>
       </c>
-      <c r="E1" s="159"/>
-      <c r="F1" s="159"/>
-      <c r="G1" s="159"/>
-      <c r="H1" s="159"/>
-      <c r="I1" s="159"/>
-      <c r="J1" s="159"/>
-      <c r="K1" s="159"/>
-      <c r="L1" s="159"/>
-      <c r="M1" s="159"/>
-      <c r="N1" s="159"/>
-      <c r="O1" s="159"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="162"/>
+      <c r="I1" s="162"/>
+      <c r="J1" s="162"/>
+      <c r="K1" s="162"/>
+      <c r="L1" s="162"/>
+      <c r="M1" s="162"/>
+      <c r="N1" s="162"/>
+      <c r="O1" s="162"/>
       <c r="P1" s="36" t="s">
         <v>284</v>
       </c>
@@ -2300,23 +2324,23 @@
     </row>
     <row r="2" spans="2:21" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G3" s="162" t="s">
+      <c r="G3" s="165" t="s">
         <v>273</v>
       </c>
-      <c r="H3" s="163"/>
-      <c r="I3" s="164"/>
-      <c r="J3" s="162" t="s">
+      <c r="H3" s="166"/>
+      <c r="I3" s="167"/>
+      <c r="J3" s="165" t="s">
         <v>274</v>
       </c>
-      <c r="K3" s="163"/>
-      <c r="L3" s="164"/>
+      <c r="K3" s="166"/>
+      <c r="L3" s="167"/>
       <c r="M3" s="76"/>
-      <c r="P3" s="156" t="s">
+      <c r="P3" s="158" t="s">
         <v>274</v>
       </c>
-      <c r="Q3" s="157"/>
-      <c r="R3" s="157"/>
-      <c r="S3" s="157"/>
+      <c r="Q3" s="159"/>
+      <c r="R3" s="159"/>
+      <c r="S3" s="159"/>
     </row>
     <row r="4" spans="2:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="27"/>
@@ -2376,7 +2400,7 @@
       </c>
     </row>
     <row r="5" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="153" t="s">
+      <c r="B5" s="156" t="s">
         <v>169</v>
       </c>
       <c r="C5" s="30">
@@ -2409,7 +2433,7 @@
       <c r="T5" s="52"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="154"/>
+      <c r="B6" s="157"/>
       <c r="C6" s="31">
         <v>2</v>
       </c>
@@ -2440,7 +2464,7 @@
       <c r="T6" s="52"/>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="154"/>
+      <c r="B7" s="157"/>
       <c r="C7" s="31">
         <v>3</v>
       </c>
@@ -2471,7 +2495,7 @@
       <c r="T7" s="52"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="154"/>
+      <c r="B8" s="157"/>
       <c r="C8" s="31">
         <v>4</v>
       </c>
@@ -2502,7 +2526,7 @@
       <c r="T8" s="52"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="154"/>
+      <c r="B9" s="157"/>
       <c r="C9" s="31">
         <v>5</v>
       </c>
@@ -2533,7 +2557,7 @@
       <c r="T9" s="52"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="154"/>
+      <c r="B10" s="157"/>
       <c r="C10" s="31">
         <v>6</v>
       </c>
@@ -2576,7 +2600,7 @@
       <c r="T10" s="52"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="154"/>
+      <c r="B11" s="157"/>
       <c r="C11" s="31">
         <v>7</v>
       </c>
@@ -2619,7 +2643,7 @@
       <c r="T11" s="52"/>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="154"/>
+      <c r="B12" s="157"/>
       <c r="C12" s="31">
         <v>8</v>
       </c>
@@ -2662,7 +2686,7 @@
       <c r="T12" s="52"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="154"/>
+      <c r="B13" s="157"/>
       <c r="C13" s="31">
         <v>9</v>
       </c>
@@ -2705,7 +2729,7 @@
       <c r="T13" s="52"/>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="154"/>
+      <c r="B14" s="157"/>
       <c r="C14" s="31">
         <v>10</v>
       </c>
@@ -2752,7 +2776,7 @@
       <c r="T14" s="52"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="154"/>
+      <c r="B15" s="157"/>
       <c r="C15" s="31">
         <v>11</v>
       </c>
@@ -2799,7 +2823,7 @@
       <c r="T15" s="52"/>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="154"/>
+      <c r="B16" s="157"/>
       <c r="C16" s="31">
         <v>12</v>
       </c>
@@ -2846,7 +2870,7 @@
       <c r="T16" s="52"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="154"/>
+      <c r="B17" s="157"/>
       <c r="C17" s="31">
         <v>13</v>
       </c>
@@ -2893,7 +2917,7 @@
       <c r="T17" s="52"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="154"/>
+      <c r="B18" s="157"/>
       <c r="C18" s="31">
         <v>14</v>
       </c>
@@ -2940,7 +2964,7 @@
       <c r="T18" s="52"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B19" s="154"/>
+      <c r="B19" s="157"/>
       <c r="C19" s="31">
         <v>15</v>
       </c>
@@ -2983,7 +3007,7 @@
       <c r="T19" s="52"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="154"/>
+      <c r="B20" s="157"/>
       <c r="C20" s="31">
         <v>16</v>
       </c>
@@ -3026,7 +3050,7 @@
       <c r="T20" s="52"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="154"/>
+      <c r="B21" s="157"/>
       <c r="C21" s="31">
         <v>17</v>
       </c>
@@ -3069,7 +3093,7 @@
       <c r="T21" s="52"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="154"/>
+      <c r="B22" s="157"/>
       <c r="C22" s="31">
         <v>18</v>
       </c>
@@ -3112,7 +3136,7 @@
       <c r="T22" s="52"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="154"/>
+      <c r="B23" s="157"/>
       <c r="C23" s="31">
         <v>19</v>
       </c>
@@ -3155,7 +3179,7 @@
       <c r="T23" s="52"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="154"/>
+      <c r="B24" s="157"/>
       <c r="C24" s="31">
         <v>20</v>
       </c>
@@ -3198,7 +3222,7 @@
       <c r="T24" s="52"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="154"/>
+      <c r="B25" s="157"/>
       <c r="C25" s="31">
         <v>21</v>
       </c>
@@ -3241,7 +3265,7 @@
       <c r="T25" s="52"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B26" s="154"/>
+      <c r="B26" s="157"/>
       <c r="C26" s="31">
         <v>22</v>
       </c>
@@ -3284,7 +3308,7 @@
       <c r="T26" s="52"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B27" s="154"/>
+      <c r="B27" s="157"/>
       <c r="C27" s="31">
         <v>23</v>
       </c>
@@ -3328,7 +3352,7 @@
       <c r="T27" s="52"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B28" s="154"/>
+      <c r="B28" s="157"/>
       <c r="C28" s="31">
         <v>24</v>
       </c>
@@ -3371,7 +3395,7 @@
       <c r="T28" s="52"/>
     </row>
     <row r="29" spans="2:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="155"/>
+      <c r="B29" s="160"/>
       <c r="C29" s="32">
         <v>25</v>
       </c>
@@ -3429,7 +3453,7 @@
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="153" t="s">
+      <c r="B30" s="156" t="s">
         <v>175</v>
       </c>
       <c r="C30" s="39">
@@ -3474,7 +3498,7 @@
       <c r="T30" s="52"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B31" s="160"/>
+      <c r="B31" s="163"/>
       <c r="C31" s="37">
         <v>27</v>
       </c>
@@ -3517,7 +3541,7 @@
       <c r="T31" s="52"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B32" s="160"/>
+      <c r="B32" s="163"/>
       <c r="C32" s="37">
         <v>28</v>
       </c>
@@ -3560,7 +3584,7 @@
       <c r="T32" s="52"/>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B33" s="160"/>
+      <c r="B33" s="163"/>
       <c r="C33" s="37">
         <v>29</v>
       </c>
@@ -3607,7 +3631,7 @@
       <c r="T33" s="52"/>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="160"/>
+      <c r="B34" s="163"/>
       <c r="C34" s="37">
         <v>30</v>
       </c>
@@ -3650,7 +3674,7 @@
       <c r="T34" s="52"/>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B35" s="160"/>
+      <c r="B35" s="163"/>
       <c r="C35" s="37">
         <v>31</v>
       </c>
@@ -3697,7 +3721,7 @@
       <c r="T35" s="52"/>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="160"/>
+      <c r="B36" s="163"/>
       <c r="C36" s="37">
         <v>32</v>
       </c>
@@ -3744,7 +3768,7 @@
       <c r="T36" s="52"/>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B37" s="160"/>
+      <c r="B37" s="163"/>
       <c r="C37" s="37">
         <v>33</v>
       </c>
@@ -3791,7 +3815,7 @@
       <c r="T37" s="52"/>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B38" s="160"/>
+      <c r="B38" s="163"/>
       <c r="C38" s="37">
         <v>34</v>
       </c>
@@ -3838,7 +3862,7 @@
       <c r="T38" s="52"/>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B39" s="160"/>
+      <c r="B39" s="163"/>
       <c r="C39" s="37">
         <v>35</v>
       </c>
@@ -3881,7 +3905,7 @@
       <c r="T39" s="52"/>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B40" s="160"/>
+      <c r="B40" s="163"/>
       <c r="C40" s="37">
         <v>36</v>
       </c>
@@ -3924,7 +3948,7 @@
       <c r="T40" s="52"/>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B41" s="160"/>
+      <c r="B41" s="163"/>
       <c r="C41" s="37">
         <v>37</v>
       </c>
@@ -3971,7 +3995,7 @@
       <c r="T41" s="52"/>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B42" s="160"/>
+      <c r="B42" s="163"/>
       <c r="C42" s="37">
         <v>38</v>
       </c>
@@ -4014,7 +4038,7 @@
       <c r="T42" s="52"/>
     </row>
     <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B43" s="160"/>
+      <c r="B43" s="163"/>
       <c r="C43" s="37">
         <v>39</v>
       </c>
@@ -4057,7 +4081,7 @@
       <c r="T43" s="52"/>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B44" s="160"/>
+      <c r="B44" s="163"/>
       <c r="C44" s="37">
         <v>40</v>
       </c>
@@ -4100,7 +4124,7 @@
       <c r="T44" s="52"/>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B45" s="160"/>
+      <c r="B45" s="163"/>
       <c r="C45" s="37">
         <v>41</v>
       </c>
@@ -4143,7 +4167,7 @@
       <c r="T45" s="52"/>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B46" s="160"/>
+      <c r="B46" s="163"/>
       <c r="C46" s="37">
         <v>42</v>
       </c>
@@ -4186,7 +4210,7 @@
       <c r="T46" s="52"/>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B47" s="160"/>
+      <c r="B47" s="163"/>
       <c r="C47" s="37">
         <v>43</v>
       </c>
@@ -4229,7 +4253,7 @@
       <c r="T47" s="52"/>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B48" s="160"/>
+      <c r="B48" s="163"/>
       <c r="C48" s="37">
         <v>44</v>
       </c>
@@ -4272,7 +4296,7 @@
       <c r="T48" s="52"/>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="160"/>
+      <c r="B49" s="163"/>
       <c r="C49" s="37">
         <v>45</v>
       </c>
@@ -4315,7 +4339,7 @@
       <c r="T49" s="52"/>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B50" s="160"/>
+      <c r="B50" s="163"/>
       <c r="C50" s="37">
         <v>46</v>
       </c>
@@ -4358,7 +4382,7 @@
       <c r="T50" s="52"/>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B51" s="160"/>
+      <c r="B51" s="163"/>
       <c r="C51" s="37">
         <v>47</v>
       </c>
@@ -4401,7 +4425,7 @@
       <c r="T51" s="52"/>
     </row>
     <row r="52" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B52" s="161"/>
+      <c r="B52" s="164"/>
       <c r="C52" s="43">
         <v>48</v>
       </c>
@@ -4459,7 +4483,7 @@
       </c>
     </row>
     <row r="53" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B53" s="153" t="s">
+      <c r="B53" s="156" t="s">
         <v>202</v>
       </c>
       <c r="C53" s="39">
@@ -4507,7 +4531,7 @@
       <c r="T53" s="52"/>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B54" s="161"/>
+      <c r="B54" s="164"/>
       <c r="C54" s="43">
         <v>50</v>
       </c>
@@ -4568,7 +4592,7 @@
       </c>
     </row>
     <row r="55" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B55" s="153" t="s">
+      <c r="B55" s="156" t="s">
         <v>169</v>
       </c>
       <c r="C55" s="39">
@@ -4612,7 +4636,7 @@
       <c r="T55" s="52"/>
     </row>
     <row r="56" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B56" s="154"/>
+      <c r="B56" s="157"/>
       <c r="C56" s="37">
         <v>52</v>
       </c>
@@ -4654,7 +4678,7 @@
       <c r="T56" s="52"/>
     </row>
     <row r="57" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B57" s="154"/>
+      <c r="B57" s="157"/>
       <c r="C57" s="37">
         <v>53</v>
       </c>
@@ -4696,7 +4720,7 @@
       <c r="T57" s="52"/>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B58" s="154"/>
+      <c r="B58" s="157"/>
       <c r="C58" s="37">
         <v>54</v>
       </c>
@@ -4738,7 +4762,7 @@
       <c r="T58" s="52"/>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B59" s="154"/>
+      <c r="B59" s="157"/>
       <c r="C59" s="37">
         <v>55</v>
       </c>
@@ -4780,7 +4804,7 @@
       <c r="T59" s="52"/>
     </row>
     <row r="60" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B60" s="154"/>
+      <c r="B60" s="157"/>
       <c r="C60" s="37">
         <v>56</v>
       </c>
@@ -4822,7 +4846,7 @@
       <c r="T60" s="52"/>
     </row>
     <row r="61" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B61" s="154"/>
+      <c r="B61" s="157"/>
       <c r="C61" s="37">
         <v>57</v>
       </c>
@@ -4864,7 +4888,7 @@
       <c r="T61" s="52"/>
     </row>
     <row r="62" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B62" s="154"/>
+      <c r="B62" s="157"/>
       <c r="C62" s="37">
         <v>58</v>
       </c>
@@ -4906,7 +4930,7 @@
       <c r="T62" s="52"/>
     </row>
     <row r="63" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B63" s="154"/>
+      <c r="B63" s="157"/>
       <c r="C63" s="37">
         <v>59</v>
       </c>
@@ -4948,7 +4972,7 @@
       <c r="T63" s="52"/>
     </row>
     <row r="64" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B64" s="154"/>
+      <c r="B64" s="157"/>
       <c r="C64" s="37">
         <v>60</v>
       </c>
@@ -4990,7 +5014,7 @@
       <c r="T64" s="52"/>
     </row>
     <row r="65" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B65" s="154"/>
+      <c r="B65" s="157"/>
       <c r="C65" s="37">
         <v>61</v>
       </c>
@@ -5032,7 +5056,7 @@
       <c r="T65" s="52"/>
     </row>
     <row r="66" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B66" s="154"/>
+      <c r="B66" s="157"/>
       <c r="C66" s="37">
         <v>62</v>
       </c>
@@ -5074,7 +5098,7 @@
       <c r="T66" s="52"/>
     </row>
     <row r="67" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B67" s="154"/>
+      <c r="B67" s="157"/>
       <c r="C67" s="37">
         <v>63</v>
       </c>
@@ -5116,7 +5140,7 @@
       <c r="T67" s="52"/>
     </row>
     <row r="68" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B68" s="154"/>
+      <c r="B68" s="157"/>
       <c r="C68" s="37">
         <v>64</v>
       </c>
@@ -5158,7 +5182,7 @@
       <c r="T68" s="52"/>
     </row>
     <row r="69" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B69" s="154"/>
+      <c r="B69" s="157"/>
       <c r="C69" s="37">
         <v>65</v>
       </c>
@@ -5200,7 +5224,7 @@
       <c r="T69" s="52"/>
     </row>
     <row r="70" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B70" s="154"/>
+      <c r="B70" s="157"/>
       <c r="C70" s="37">
         <v>66</v>
       </c>
@@ -5242,7 +5266,7 @@
       <c r="T70" s="52"/>
     </row>
     <row r="71" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B71" s="154"/>
+      <c r="B71" s="157"/>
       <c r="C71" s="37">
         <v>67</v>
       </c>
@@ -5284,7 +5308,7 @@
       <c r="T71" s="52"/>
     </row>
     <row r="72" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B72" s="154"/>
+      <c r="B72" s="157"/>
       <c r="C72" s="37">
         <v>68</v>
       </c>
@@ -5326,7 +5350,7 @@
       <c r="T72" s="52"/>
     </row>
     <row r="73" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B73" s="154"/>
+      <c r="B73" s="157"/>
       <c r="C73" s="37">
         <v>69</v>
       </c>
@@ -5370,7 +5394,7 @@
       <c r="T73" s="52"/>
     </row>
     <row r="74" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B74" s="154"/>
+      <c r="B74" s="157"/>
       <c r="C74" s="37">
         <v>70</v>
       </c>
@@ -5412,7 +5436,7 @@
       <c r="T74" s="52"/>
     </row>
     <row r="75" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B75" s="154"/>
+      <c r="B75" s="157"/>
       <c r="C75" s="37">
         <v>71</v>
       </c>
@@ -5454,7 +5478,7 @@
       <c r="T75" s="52"/>
     </row>
     <row r="76" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B76" s="154"/>
+      <c r="B76" s="157"/>
       <c r="C76" s="37">
         <v>72</v>
       </c>
@@ -5496,7 +5520,7 @@
       <c r="T76" s="52"/>
     </row>
     <row r="77" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B77" s="154"/>
+      <c r="B77" s="157"/>
       <c r="C77" s="37">
         <v>73</v>
       </c>
@@ -5538,7 +5562,7 @@
       <c r="T77" s="52"/>
     </row>
     <row r="78" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B78" s="154"/>
+      <c r="B78" s="157"/>
       <c r="C78" s="37">
         <v>74</v>
       </c>
@@ -5580,7 +5604,7 @@
       <c r="T78" s="52"/>
     </row>
     <row r="79" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B79" s="155"/>
+      <c r="B79" s="160"/>
       <c r="C79" s="43">
         <v>75</v>
       </c>
@@ -5639,7 +5663,7 @@
       </c>
     </row>
     <row r="80" spans="2:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="153" t="s">
+      <c r="B80" s="156" t="s">
         <v>276</v>
       </c>
       <c r="C80" s="39">
@@ -5683,7 +5707,7 @@
       <c r="T80" s="52"/>
     </row>
     <row r="81" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B81" s="154"/>
+      <c r="B81" s="157"/>
       <c r="C81" s="37">
         <v>77</v>
       </c>
@@ -5725,7 +5749,7 @@
       <c r="T81" s="52"/>
     </row>
     <row r="82" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B82" s="154"/>
+      <c r="B82" s="157"/>
       <c r="C82" s="37">
         <v>78</v>
       </c>
@@ -5767,7 +5791,7 @@
       <c r="T82" s="52"/>
     </row>
     <row r="83" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B83" s="154"/>
+      <c r="B83" s="157"/>
       <c r="C83" s="37">
         <v>79</v>
       </c>
@@ -5809,7 +5833,7 @@
       <c r="T83" s="52"/>
     </row>
     <row r="84" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B84" s="154"/>
+      <c r="B84" s="157"/>
       <c r="C84" s="37">
         <v>80</v>
       </c>
@@ -5851,7 +5875,7 @@
       <c r="T84" s="52"/>
     </row>
     <row r="85" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B85" s="154"/>
+      <c r="B85" s="157"/>
       <c r="C85" s="37">
         <v>81</v>
       </c>
@@ -5895,7 +5919,7 @@
       <c r="T85" s="52"/>
     </row>
     <row r="86" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B86" s="154"/>
+      <c r="B86" s="157"/>
       <c r="C86" s="37">
         <v>82</v>
       </c>
@@ -5937,7 +5961,7 @@
       <c r="T86" s="52"/>
     </row>
     <row r="87" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B87" s="154"/>
+      <c r="B87" s="157"/>
       <c r="C87" s="37">
         <v>83</v>
       </c>
@@ -5979,7 +6003,7 @@
       <c r="T87" s="52"/>
     </row>
     <row r="88" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B88" s="154"/>
+      <c r="B88" s="157"/>
       <c r="C88" s="37">
         <v>84</v>
       </c>
@@ -6021,7 +6045,7 @@
       <c r="T88" s="52"/>
     </row>
     <row r="89" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B89" s="154"/>
+      <c r="B89" s="157"/>
       <c r="C89" s="37">
         <v>85</v>
       </c>
@@ -6063,7 +6087,7 @@
       <c r="T89" s="52"/>
     </row>
     <row r="90" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B90" s="154"/>
+      <c r="B90" s="157"/>
       <c r="C90" s="37">
         <v>86</v>
       </c>
@@ -6105,7 +6129,7 @@
       <c r="T90" s="52"/>
     </row>
     <row r="91" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B91" s="154"/>
+      <c r="B91" s="157"/>
       <c r="C91" s="37">
         <v>87</v>
       </c>
@@ -6149,7 +6173,7 @@
       <c r="T91" s="52"/>
     </row>
     <row r="92" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B92" s="154"/>
+      <c r="B92" s="157"/>
       <c r="C92" s="37">
         <v>88</v>
       </c>
@@ -6191,7 +6215,7 @@
       <c r="T92" s="52"/>
     </row>
     <row r="93" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B93" s="154"/>
+      <c r="B93" s="157"/>
       <c r="C93" s="37">
         <v>89</v>
       </c>
@@ -6233,7 +6257,7 @@
       <c r="T93" s="52"/>
     </row>
     <row r="94" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B94" s="154"/>
+      <c r="B94" s="157"/>
       <c r="C94" s="37">
         <v>90</v>
       </c>
@@ -6275,7 +6299,7 @@
       <c r="T94" s="52"/>
     </row>
     <row r="95" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B95" s="154"/>
+      <c r="B95" s="157"/>
       <c r="C95" s="37">
         <v>91</v>
       </c>
@@ -6317,7 +6341,7 @@
       <c r="T95" s="52"/>
     </row>
     <row r="96" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B96" s="154"/>
+      <c r="B96" s="157"/>
       <c r="C96" s="37">
         <v>92</v>
       </c>
@@ -6359,7 +6383,7 @@
       <c r="T96" s="52"/>
     </row>
     <row r="97" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B97" s="154"/>
+      <c r="B97" s="157"/>
       <c r="C97" s="37">
         <v>93</v>
       </c>
@@ -6401,7 +6425,7 @@
       <c r="T97" s="52"/>
     </row>
     <row r="98" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B98" s="154"/>
+      <c r="B98" s="157"/>
       <c r="C98" s="37">
         <v>94</v>
       </c>
@@ -6443,7 +6467,7 @@
       <c r="T98" s="52"/>
     </row>
     <row r="99" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B99" s="154"/>
+      <c r="B99" s="157"/>
       <c r="C99" s="37">
         <v>95</v>
       </c>
@@ -6485,7 +6509,7 @@
       <c r="T99" s="52"/>
     </row>
     <row r="100" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B100" s="154"/>
+      <c r="B100" s="157"/>
       <c r="C100" s="37">
         <v>96</v>
       </c>
@@ -6527,7 +6551,7 @@
       <c r="T100" s="52"/>
     </row>
     <row r="101" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B101" s="154"/>
+      <c r="B101" s="157"/>
       <c r="C101" s="37">
         <v>97</v>
       </c>
@@ -6569,7 +6593,7 @@
       <c r="T101" s="52"/>
     </row>
     <row r="102" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B102" s="154"/>
+      <c r="B102" s="157"/>
       <c r="C102" s="37">
         <v>98</v>
       </c>
@@ -6611,7 +6635,7 @@
       <c r="T102" s="52"/>
     </row>
     <row r="103" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B103" s="154"/>
+      <c r="B103" s="157"/>
       <c r="C103" s="37">
         <v>99</v>
       </c>
@@ -6652,7 +6676,7 @@
       <c r="T103" s="52"/>
     </row>
     <row r="104" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B104" s="154"/>
+      <c r="B104" s="157"/>
       <c r="C104" s="37">
         <v>100</v>
       </c>
@@ -6693,7 +6717,7 @@
       <c r="T104" s="52"/>
     </row>
     <row r="105" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B105" s="155"/>
+      <c r="B105" s="160"/>
       <c r="C105" s="43">
         <v>101</v>
       </c>
@@ -6749,7 +6773,7 @@
       </c>
     </row>
     <row r="106" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B106" s="153" t="s">
+      <c r="B106" s="156" t="s">
         <v>263</v>
       </c>
       <c r="C106" s="39">
@@ -6792,7 +6816,7 @@
       <c r="T106" s="52"/>
     </row>
     <row r="107" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B107" s="154"/>
+      <c r="B107" s="157"/>
       <c r="C107" s="37">
         <v>103</v>
       </c>
@@ -6833,7 +6857,7 @@
       <c r="T107" s="52"/>
     </row>
     <row r="108" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B108" s="154"/>
+      <c r="B108" s="157"/>
       <c r="C108" s="37">
         <v>104</v>
       </c>
@@ -6874,7 +6898,7 @@
       <c r="T108" s="52"/>
     </row>
     <row r="109" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B109" s="154"/>
+      <c r="B109" s="157"/>
       <c r="C109" s="37">
         <v>105</v>
       </c>
@@ -6915,7 +6939,7 @@
       <c r="T109" s="52"/>
     </row>
     <row r="110" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B110" s="154"/>
+      <c r="B110" s="157"/>
       <c r="C110" s="37">
         <v>106</v>
       </c>
@@ -6956,7 +6980,7 @@
       <c r="T110" s="52"/>
     </row>
     <row r="111" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B111" s="154"/>
+      <c r="B111" s="157"/>
       <c r="C111" s="37">
         <v>107</v>
       </c>
@@ -6997,7 +7021,7 @@
       <c r="T111" s="52"/>
     </row>
     <row r="112" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B112" s="154"/>
+      <c r="B112" s="157"/>
       <c r="C112" s="37">
         <v>108</v>
       </c>
@@ -7038,7 +7062,7 @@
       <c r="T112" s="52"/>
     </row>
     <row r="113" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B113" s="155"/>
+      <c r="B113" s="160"/>
       <c r="C113" s="43">
         <v>109</v>
       </c>
@@ -7093,7 +7117,7 @@
       </c>
     </row>
     <row r="114" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B114" s="153" t="s">
+      <c r="B114" s="156" t="s">
         <v>169</v>
       </c>
       <c r="C114" s="39">
@@ -7132,7 +7156,7 @@
       <c r="T114" s="52"/>
     </row>
     <row r="115" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B115" s="154"/>
+      <c r="B115" s="157"/>
       <c r="C115" s="37">
         <v>111</v>
       </c>
@@ -7169,7 +7193,7 @@
       <c r="T115" s="52"/>
     </row>
     <row r="116" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B116" s="154"/>
+      <c r="B116" s="157"/>
       <c r="C116" s="37">
         <v>112</v>
       </c>
@@ -7206,7 +7230,7 @@
       <c r="T116" s="52"/>
     </row>
     <row r="117" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B117" s="154"/>
+      <c r="B117" s="157"/>
       <c r="C117" s="37">
         <v>113</v>
       </c>
@@ -7243,7 +7267,7 @@
       <c r="T117" s="52"/>
     </row>
     <row r="118" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B118" s="154"/>
+      <c r="B118" s="157"/>
       <c r="C118" s="37">
         <v>114</v>
       </c>
@@ -7280,7 +7304,7 @@
       <c r="T118" s="52"/>
     </row>
     <row r="119" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B119" s="154"/>
+      <c r="B119" s="157"/>
       <c r="C119" s="37">
         <v>115</v>
       </c>
@@ -7317,7 +7341,7 @@
       <c r="T119" s="52"/>
     </row>
     <row r="120" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B120" s="154"/>
+      <c r="B120" s="157"/>
       <c r="C120" s="37">
         <v>116</v>
       </c>
@@ -7354,7 +7378,7 @@
       <c r="T120" s="52"/>
     </row>
     <row r="121" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B121" s="154"/>
+      <c r="B121" s="157"/>
       <c r="C121" s="37">
         <v>117</v>
       </c>
@@ -7391,7 +7415,7 @@
       <c r="T121" s="52"/>
     </row>
     <row r="122" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B122" s="154"/>
+      <c r="B122" s="157"/>
       <c r="C122" s="37">
         <v>118</v>
       </c>
@@ -7428,7 +7452,7 @@
       <c r="T122" s="52"/>
     </row>
     <row r="123" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B123" s="154"/>
+      <c r="B123" s="157"/>
       <c r="C123" s="37">
         <v>119</v>
       </c>
@@ -7465,7 +7489,7 @@
       <c r="T123" s="52"/>
     </row>
     <row r="124" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B124" s="154"/>
+      <c r="B124" s="157"/>
       <c r="C124" s="37">
         <v>120</v>
       </c>
@@ -7502,7 +7526,7 @@
       <c r="T124" s="52"/>
     </row>
     <row r="125" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B125" s="154"/>
+      <c r="B125" s="157"/>
       <c r="C125" s="37">
         <v>121</v>
       </c>
@@ -7539,7 +7563,7 @@
       <c r="T125" s="52"/>
     </row>
     <row r="126" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B126" s="154"/>
+      <c r="B126" s="157"/>
       <c r="C126" s="37">
         <v>122</v>
       </c>
@@ -7576,7 +7600,7 @@
       <c r="T126" s="52"/>
     </row>
     <row r="127" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B127" s="154"/>
+      <c r="B127" s="157"/>
       <c r="C127" s="37">
         <v>123</v>
       </c>
@@ -7613,7 +7637,7 @@
       <c r="T127" s="52"/>
     </row>
     <row r="128" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B128" s="154"/>
+      <c r="B128" s="157"/>
       <c r="C128" s="37">
         <v>124</v>
       </c>
@@ -7650,7 +7674,7 @@
       <c r="T128" s="52"/>
     </row>
     <row r="129" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B129" s="154"/>
+      <c r="B129" s="157"/>
       <c r="C129" s="37">
         <v>125</v>
       </c>
@@ -7687,7 +7711,7 @@
       <c r="T129" s="52"/>
     </row>
     <row r="130" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B130" s="154"/>
+      <c r="B130" s="157"/>
       <c r="C130" s="37">
         <v>126</v>
       </c>
@@ -7724,7 +7748,7 @@
       <c r="T130" s="52"/>
     </row>
     <row r="131" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B131" s="154"/>
+      <c r="B131" s="157"/>
       <c r="C131" s="37">
         <v>127</v>
       </c>
@@ -7761,7 +7785,7 @@
       <c r="T131" s="52"/>
     </row>
     <row r="132" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B132" s="154"/>
+      <c r="B132" s="157"/>
       <c r="C132" s="37">
         <v>128</v>
       </c>
@@ -7798,7 +7822,7 @@
       <c r="T132" s="52"/>
     </row>
     <row r="133" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B133" s="154"/>
+      <c r="B133" s="157"/>
       <c r="C133" s="37">
         <v>129</v>
       </c>
@@ -7835,7 +7859,7 @@
       <c r="T133" s="52"/>
     </row>
     <row r="134" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B134" s="154"/>
+      <c r="B134" s="157"/>
       <c r="C134" s="37">
         <v>130</v>
       </c>
@@ -7872,7 +7896,7 @@
       <c r="T134" s="52"/>
     </row>
     <row r="135" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B135" s="154"/>
+      <c r="B135" s="157"/>
       <c r="C135" s="37">
         <v>131</v>
       </c>
@@ -7911,7 +7935,7 @@
       <c r="T135" s="52"/>
     </row>
     <row r="136" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B136" s="154"/>
+      <c r="B136" s="157"/>
       <c r="C136" s="37">
         <v>132</v>
       </c>
@@ -7950,7 +7974,7 @@
       <c r="T136" s="52"/>
     </row>
     <row r="137" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B137" s="154"/>
+      <c r="B137" s="157"/>
       <c r="C137" s="37">
         <v>133</v>
       </c>
@@ -7987,7 +8011,7 @@
       <c r="T137" s="52"/>
     </row>
     <row r="138" spans="2:20" s="116" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="155"/>
+      <c r="B138" s="160"/>
       <c r="C138" s="43">
         <v>134</v>
       </c>
@@ -8037,8 +8061,10 @@
         <v>275</v>
       </c>
     </row>
-    <row r="139" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B139" s="153"/>
+    <row r="139" spans="2:20" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="156" t="s">
+        <v>369</v>
+      </c>
       <c r="C139" s="39">
         <v>135</v>
       </c>
@@ -8073,7 +8099,7 @@
       <c r="T139" s="52"/>
     </row>
     <row r="140" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B140" s="154"/>
+      <c r="B140" s="157"/>
       <c r="C140" s="37">
         <v>136</v>
       </c>
@@ -8108,7 +8134,7 @@
       <c r="T140" s="52"/>
     </row>
     <row r="141" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B141" s="154"/>
+      <c r="B141" s="157"/>
       <c r="C141" s="37">
         <v>137</v>
       </c>
@@ -8143,7 +8169,7 @@
       <c r="T141" s="52"/>
     </row>
     <row r="142" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B142" s="154"/>
+      <c r="B142" s="157"/>
       <c r="C142" s="37">
         <v>138</v>
       </c>
@@ -8178,7 +8204,7 @@
       <c r="T142" s="52"/>
     </row>
     <row r="143" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B143" s="154"/>
+      <c r="B143" s="157"/>
       <c r="C143" s="37">
         <v>139</v>
       </c>
@@ -8213,7 +8239,7 @@
       <c r="T143" s="52"/>
     </row>
     <row r="144" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B144" s="154"/>
+      <c r="B144" s="157"/>
       <c r="C144" s="37">
         <v>140</v>
       </c>
@@ -8248,7 +8274,7 @@
       <c r="T144" s="52"/>
     </row>
     <row r="145" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B145" s="154"/>
+      <c r="B145" s="157"/>
       <c r="C145" s="37">
         <v>141</v>
       </c>
@@ -8283,7 +8309,7 @@
       <c r="T145" s="52"/>
     </row>
     <row r="146" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B146" s="154"/>
+      <c r="B146" s="157"/>
       <c r="C146" s="37">
         <v>142</v>
       </c>
@@ -8318,7 +8344,7 @@
       <c r="T146" s="52"/>
     </row>
     <row r="147" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B147" s="154"/>
+      <c r="B147" s="157"/>
       <c r="C147" s="37">
         <v>143</v>
       </c>
@@ -8353,7 +8379,7 @@
       <c r="T147" s="52"/>
     </row>
     <row r="148" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B148" s="154"/>
+      <c r="B148" s="157"/>
       <c r="C148" s="37">
         <v>144</v>
       </c>
@@ -8388,7 +8414,7 @@
       <c r="T148" s="52"/>
     </row>
     <row r="149" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B149" s="154"/>
+      <c r="B149" s="157"/>
       <c r="C149" s="37">
         <v>145</v>
       </c>
@@ -8423,7 +8449,7 @@
       <c r="T149" s="52"/>
     </row>
     <row r="150" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B150" s="154"/>
+      <c r="B150" s="157"/>
       <c r="C150" s="37">
         <v>146</v>
       </c>
@@ -8458,7 +8484,7 @@
       <c r="T150" s="52"/>
     </row>
     <row r="151" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B151" s="154"/>
+      <c r="B151" s="157"/>
       <c r="C151" s="37">
         <v>147</v>
       </c>
@@ -8493,7 +8519,7 @@
       <c r="T151" s="52"/>
     </row>
     <row r="152" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B152" s="154"/>
+      <c r="B152" s="157"/>
       <c r="C152" s="37">
         <v>148</v>
       </c>
@@ -8528,7 +8554,7 @@
       <c r="T152" s="52"/>
     </row>
     <row r="153" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B153" s="154"/>
+      <c r="B153" s="157"/>
       <c r="C153" s="37">
         <v>149</v>
       </c>
@@ -8563,7 +8589,7 @@
       <c r="T153" s="52"/>
     </row>
     <row r="154" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B154" s="154"/>
+      <c r="B154" s="157"/>
       <c r="C154" s="37">
         <v>150</v>
       </c>
@@ -8598,7 +8624,7 @@
       <c r="T154" s="52"/>
     </row>
     <row r="155" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B155" s="154"/>
+      <c r="B155" s="157"/>
       <c r="C155" s="37">
         <v>151</v>
       </c>
@@ -8633,7 +8659,7 @@
       <c r="T155" s="52"/>
     </row>
     <row r="156" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B156" s="154"/>
+      <c r="B156" s="157"/>
       <c r="C156" s="37">
         <v>152</v>
       </c>
@@ -8668,7 +8694,7 @@
       <c r="T156" s="52"/>
     </row>
     <row r="157" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B157" s="154"/>
+      <c r="B157" s="157"/>
       <c r="C157" s="37">
         <v>153</v>
       </c>
@@ -8703,7 +8729,7 @@
       <c r="T157" s="52"/>
     </row>
     <row r="158" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B158" s="154"/>
+      <c r="B158" s="157"/>
       <c r="C158" s="37">
         <v>154</v>
       </c>
@@ -8738,7 +8764,7 @@
       <c r="T158" s="52"/>
     </row>
     <row r="159" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B159" s="154"/>
+      <c r="B159" s="157"/>
       <c r="C159" s="37">
         <v>155</v>
       </c>
@@ -8773,12 +8799,12 @@
       <c r="T159" s="52"/>
     </row>
     <row r="160" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B160" s="154"/>
+      <c r="B160" s="157"/>
       <c r="C160" s="37">
         <v>156</v>
       </c>
       <c r="D160" s="38" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E160" s="19" t="s">
         <v>365</v>
@@ -8808,7 +8834,7 @@
       <c r="T160" s="52"/>
     </row>
     <row r="161" spans="2:20" s="116" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B161" s="154"/>
+      <c r="B161" s="160"/>
       <c r="C161" s="43">
         <v>157</v>
       </c>
@@ -8828,7 +8854,7 @@
       <c r="K161" s="46">
         <v>231</v>
       </c>
-      <c r="L161" s="167">
+      <c r="L161" s="153">
         <v>94.7</v>
       </c>
       <c r="M161" s="147" t="s">
@@ -8854,125 +8880,255 @@
       </c>
       <c r="T161" s="148"/>
     </row>
-    <row r="162" spans="2:20" s="98" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="97"/>
-      <c r="E162" s="99"/>
-      <c r="I162" s="100"/>
-      <c r="J162" s="101"/>
-      <c r="K162" s="168">
-        <f>SUM(K10:K161)</f>
-        <v>33893</v>
-      </c>
-      <c r="L162" s="169">
-        <f>AVERAGE(L10:L161)</f>
-        <v>91.387499999999932</v>
-      </c>
-      <c r="M162" s="100"/>
-      <c r="N162" s="102"/>
-      <c r="O162" s="103" t="s">
+    <row r="162" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B162" s="156" t="s">
+        <v>370</v>
+      </c>
+      <c r="C162" s="37">
+        <v>154</v>
+      </c>
+      <c r="D162" s="38" t="s">
+        <v>375</v>
+      </c>
+      <c r="E162" s="19" t="s">
+        <v>371</v>
+      </c>
+      <c r="F162" s="1"/>
+      <c r="G162" s="1"/>
+      <c r="H162" s="42"/>
+      <c r="I162" s="11"/>
+      <c r="J162" s="90">
+        <v>42272</v>
+      </c>
+      <c r="K162" s="42">
+        <v>213</v>
+      </c>
+      <c r="L162" s="80">
+        <v>87.3</v>
+      </c>
+      <c r="M162" s="83" t="s">
+        <v>275</v>
+      </c>
+      <c r="N162" s="48"/>
+      <c r="O162" s="62"/>
+      <c r="P162" s="51"/>
+      <c r="Q162" s="1"/>
+      <c r="R162" s="1"/>
+      <c r="S162" s="52"/>
+      <c r="T162" s="52"/>
+    </row>
+    <row r="163" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B163" s="157"/>
+      <c r="C163" s="37">
+        <v>155</v>
+      </c>
+      <c r="D163" s="38" t="s">
+        <v>375</v>
+      </c>
+      <c r="E163" s="19" t="s">
+        <v>372</v>
+      </c>
+      <c r="F163" s="1"/>
+      <c r="G163" s="1"/>
+      <c r="H163" s="42"/>
+      <c r="I163" s="11"/>
+      <c r="J163" s="90">
+        <v>42271</v>
+      </c>
+      <c r="K163" s="42">
+        <v>230</v>
+      </c>
+      <c r="L163" s="80">
+        <v>94.3</v>
+      </c>
+      <c r="M163" s="83" t="s">
+        <v>275</v>
+      </c>
+      <c r="N163" s="48"/>
+      <c r="O163" s="61"/>
+      <c r="P163" s="51"/>
+      <c r="Q163" s="1"/>
+      <c r="R163" s="1"/>
+      <c r="S163" s="52"/>
+      <c r="T163" s="52"/>
+    </row>
+    <row r="164" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B164" s="157"/>
+      <c r="C164" s="37">
+        <v>156</v>
+      </c>
+      <c r="D164" s="38" t="s">
+        <v>375</v>
+      </c>
+      <c r="E164" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="F164" s="1"/>
+      <c r="G164" s="1"/>
+      <c r="H164" s="42"/>
+      <c r="I164" s="11"/>
+      <c r="J164" s="90">
+        <v>42271</v>
+      </c>
+      <c r="K164" s="42">
+        <v>216</v>
+      </c>
+      <c r="L164" s="80">
+        <v>88.5</v>
+      </c>
+      <c r="M164" s="83" t="s">
+        <v>275</v>
+      </c>
+      <c r="N164" s="48"/>
+      <c r="O164" s="61"/>
+      <c r="P164" s="51"/>
+      <c r="Q164" s="1"/>
+      <c r="R164" s="1"/>
+      <c r="S164" s="52"/>
+      <c r="T164" s="52"/>
+    </row>
+    <row r="165" spans="2:20" s="116" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B165" s="160"/>
+      <c r="C165" s="43">
+        <v>157</v>
+      </c>
+      <c r="D165" s="44" t="s">
+        <v>375</v>
+      </c>
+      <c r="E165" s="18" t="s">
+        <v>374</v>
+      </c>
+      <c r="F165" s="2"/>
+      <c r="G165" s="2"/>
+      <c r="H165" s="46"/>
+      <c r="I165" s="45"/>
+      <c r="J165" s="91">
+        <v>42271</v>
+      </c>
+      <c r="K165" s="46">
+        <v>203</v>
+      </c>
+      <c r="L165" s="173">
+        <v>83.2</v>
+      </c>
+      <c r="M165" s="147" t="s">
+        <v>275</v>
+      </c>
+      <c r="N165" s="152"/>
+      <c r="O165" s="63"/>
+      <c r="P165" s="58">
+        <f>AVERAGE(L162:L165)</f>
+        <v>88.325000000000003</v>
+      </c>
+      <c r="Q165" s="59">
+        <f>SUM(L162:L165)</f>
+        <v>353.3</v>
+      </c>
+      <c r="R165" s="58">
+        <f>MAX(L162:L165)</f>
+        <v>94.3</v>
+      </c>
+      <c r="S165" s="60">
+        <f>MIN(L162:L165)</f>
+        <v>83.2</v>
+      </c>
+      <c r="T165" s="148"/>
+    </row>
+    <row r="166" spans="2:20" s="98" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B166" s="97"/>
+      <c r="E166" s="99"/>
+      <c r="I166" s="100"/>
+      <c r="J166" s="101"/>
+      <c r="K166" s="170">
+        <f>SUM(K10:K165)</f>
+        <v>34755</v>
+      </c>
+      <c r="L166" s="171">
+        <f>AVERAGE(L10:L165)</f>
+        <v>91.308974358974282</v>
+      </c>
+      <c r="M166" s="100"/>
+      <c r="N166" s="102"/>
+      <c r="O166" s="103" t="s">
         <v>258</v>
       </c>
-      <c r="P162" s="142">
-        <f>AVERAGE(P5:P161)</f>
-        <v>91.432427675585288</v>
-      </c>
-      <c r="Q162" s="143">
-        <f>SUM(Q5:Q161)</f>
-        <v>33893</v>
-      </c>
-      <c r="R162" s="144">
-        <f>MAX(R5:R161)</f>
+      <c r="P166" s="142">
+        <f>AVERAGE(P5:P165)</f>
+        <v>91.087157933853589</v>
+      </c>
+      <c r="Q166" s="143">
+        <f>SUM(Q5:Q165)</f>
+        <v>34246.300000000003</v>
+      </c>
+      <c r="R166" s="144">
+        <f>MAX(R5:R165)</f>
         <v>98.4</v>
       </c>
-      <c r="S162" s="145">
-        <f>MIN(S5:S161)</f>
+      <c r="S166" s="145">
+        <f>MIN(S5:S165)</f>
         <v>66.8</v>
       </c>
-      <c r="T162" s="142">
+      <c r="T166" s="142">
         <f>AVERAGE(T5:T113)</f>
         <v>-1.3365161796151077</v>
       </c>
     </row>
-    <row r="163" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="E163" s="49"/>
-      <c r="F163" s="9"/>
-      <c r="G163" s="50"/>
-      <c r="J163" s="170" t="s">
-        <v>369</v>
-      </c>
-      <c r="K163" s="9">
-        <f>K162/16</f>
-        <v>2118.3125</v>
-      </c>
-    </row>
-    <row r="164" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="E164" s="49"/>
-      <c r="F164" s="9"/>
-      <c r="G164" s="50"/>
-      <c r="H164" s="68"/>
-    </row>
-    <row r="165" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="E165" s="49"/>
-      <c r="F165" s="67"/>
-      <c r="G165" s="50"/>
-      <c r="H165" s="68"/>
-      <c r="K165" s="67"/>
-    </row>
-    <row r="166" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="E166" s="49"/>
-      <c r="F166" s="67"/>
-      <c r="G166" s="50"/>
-      <c r="H166" s="68"/>
-      <c r="K166" s="67"/>
-    </row>
     <row r="167" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E167" s="49"/>
-      <c r="F167" s="67"/>
+      <c r="F167" s="9"/>
       <c r="G167" s="50"/>
-      <c r="H167" s="68"/>
-      <c r="K167" s="67"/>
+      <c r="J167" s="154" t="s">
+        <v>368</v>
+      </c>
+      <c r="K167" s="172">
+        <f>K166/16</f>
+        <v>2172.1875</v>
+      </c>
     </row>
     <row r="168" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="F168" s="68"/>
-      <c r="G168" s="68"/>
+      <c r="E168" s="49"/>
+      <c r="F168" s="9"/>
+      <c r="G168" s="50"/>
       <c r="H168" s="68"/>
-      <c r="K168" s="67"/>
     </row>
     <row r="169" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="F169" s="68"/>
-      <c r="G169" s="68"/>
+      <c r="E169" s="49"/>
+      <c r="F169" s="67"/>
+      <c r="G169" s="50"/>
       <c r="H169" s="68"/>
       <c r="K169" s="67"/>
     </row>
     <row r="170" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C170" s="20"/>
-      <c r="D170" s="66"/>
-      <c r="F170" s="68"/>
-      <c r="G170" s="68"/>
+      <c r="E170" s="49"/>
+      <c r="F170" s="67"/>
+      <c r="G170" s="50"/>
       <c r="H170" s="68"/>
       <c r="K170" s="67"/>
     </row>
     <row r="171" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="F171" s="68"/>
+      <c r="E171" s="49"/>
+      <c r="F171" s="67"/>
       <c r="G171" s="50"/>
       <c r="H171" s="68"/>
       <c r="K171" s="67"/>
     </row>
     <row r="172" spans="2:20" x14ac:dyDescent="0.25">
       <c r="F172" s="68"/>
-      <c r="G172" s="50"/>
+      <c r="G172" s="68"/>
       <c r="H172" s="68"/>
       <c r="K172" s="67"/>
     </row>
     <row r="173" spans="2:20" x14ac:dyDescent="0.25">
       <c r="F173" s="68"/>
-      <c r="G173" s="50"/>
+      <c r="G173" s="68"/>
       <c r="H173" s="68"/>
       <c r="K173" s="67"/>
     </row>
     <row r="174" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C174" s="20"/>
+      <c r="D174" s="66"/>
       <c r="F174" s="68"/>
-      <c r="G174" s="50"/>
+      <c r="G174" s="68"/>
       <c r="H174" s="68"/>
       <c r="K174" s="67"/>
     </row>
@@ -9058,51 +9214,76 @@
       <c r="F188" s="68"/>
       <c r="G188" s="50"/>
       <c r="H188" s="68"/>
-      <c r="K188" s="146"/>
+      <c r="K188" s="67"/>
     </row>
     <row r="189" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F189" s="68"/>
       <c r="G189" s="50"/>
-      <c r="K189" s="146"/>
+      <c r="H189" s="68"/>
+      <c r="K189" s="67"/>
     </row>
     <row r="190" spans="6:11" x14ac:dyDescent="0.25">
       <c r="F190" s="68"/>
       <c r="G190" s="50"/>
+      <c r="H190" s="68"/>
+      <c r="K190" s="67"/>
     </row>
     <row r="191" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F191" s="68"/>
       <c r="G191" s="50"/>
+      <c r="H191" s="68"/>
+      <c r="K191" s="67"/>
     </row>
     <row r="192" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F192" s="68"/>
       <c r="G192" s="50"/>
-    </row>
-    <row r="193" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="H192" s="68"/>
+      <c r="K192" s="146"/>
+    </row>
+    <row r="193" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F193" s="68"/>
       <c r="G193" s="50"/>
-    </row>
-    <row r="194" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="K193" s="146"/>
+    </row>
+    <row r="194" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="F194" s="68"/>
       <c r="G194" s="50"/>
-      <c r="H194" s="50"/>
-      <c r="K194" s="70"/>
-    </row>
-    <row r="195" spans="7:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="195" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G195" s="50"/>
     </row>
-    <row r="196" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G196" s="50"/>
     </row>
-    <row r="197" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G197" s="50"/>
     </row>
-    <row r="198" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G198" s="50"/>
-    </row>
-    <row r="199" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="H198" s="50"/>
+      <c r="K198" s="70"/>
+    </row>
+    <row r="199" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G199" s="50"/>
     </row>
-    <row r="200" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="6:11" x14ac:dyDescent="0.25">
       <c r="G200" s="50"/>
     </row>
+    <row r="201" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="G201" s="50"/>
+    </row>
+    <row r="202" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="G202" s="50"/>
+    </row>
+    <row r="203" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="G203" s="50"/>
+    </row>
+    <row r="204" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="G204" s="50"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="B162:B165"/>
     <mergeCell ref="B139:B161"/>
     <mergeCell ref="P3:S3"/>
     <mergeCell ref="B106:B113"/>
@@ -9129,13 +9310,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S62"/>
+  <dimension ref="A1:U62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="K8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9157,11 +9338,13 @@
     <col min="16" max="16" width="12.44140625" style="109" customWidth="1"/>
     <col min="17" max="17" width="11.44140625" style="9" customWidth="1"/>
     <col min="18" max="18" width="11.44140625" style="109" customWidth="1"/>
-    <col min="19" max="19" width="11.44140625" style="9" customWidth="1"/>
-    <col min="20" max="250" width="11.44140625" customWidth="1"/>
+    <col min="19" max="19" width="11.44140625" style="75" customWidth="1"/>
+    <col min="20" max="20" width="12.44140625" style="76" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" style="9" customWidth="1"/>
+    <col min="22" max="250" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="117" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="119"/>
       <c r="C1" s="107" t="s">
         <v>289</v>
@@ -9197,15 +9380,19 @@
       <c r="R1" s="112" t="s">
         <v>367</v>
       </c>
-      <c r="S1" s="12"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S1" s="111"/>
+      <c r="T1" s="119" t="s">
+        <v>375</v>
+      </c>
+      <c r="U1" s="12"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="107" t="s">
         <v>290</v>
       </c>
       <c r="B2" s="118">
         <f>SUM(C2:AA2)</f>
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D2" s="109">
         <v>20</v>
@@ -9231,15 +9418,18 @@
       <c r="R2" s="109">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" s="105" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T2" s="76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="105" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="108" t="s">
         <v>285</v>
       </c>
-      <c r="B3" s="165" t="s">
+      <c r="B3" s="168" t="s">
         <v>291</v>
       </c>
-      <c r="C3" s="166"/>
+      <c r="C3" s="169"/>
       <c r="D3" s="110" t="s">
         <v>286</v>
       </c>
@@ -9285,21 +9475,27 @@
       <c r="R3" s="110" t="s">
         <v>286</v>
       </c>
-      <c r="S3" s="104" t="s">
+      <c r="S3" s="106" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3" s="104" t="s">
+        <v>286</v>
+      </c>
+      <c r="U3" s="104" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="107">
         <v>0</v>
       </c>
       <c r="B4" s="121">
-        <f t="shared" ref="B4:B5" si="0">D4+F4+H4+J4+L4+N4+P4+R4</f>
-        <v>250</v>
+        <f>D4+F4+H4+J4+L4+N4+P4+R4+T4</f>
+        <v>260</v>
       </c>
       <c r="C4" s="124">
-        <f t="shared" ref="C4:C5" si="1">AVERAGE(E4,G4,I4,K4,M4,O4,Q4,S4)/100</f>
-        <v>6.3714285714285713E-3</v>
+        <f>AVERAGE(E4,G4,I4,K4,M4,O4,Q4,S4,U4)/100</f>
+        <v>6.8500000000000002E-3</v>
       </c>
       <c r="D4" s="109">
         <v>44</v>
@@ -9346,21 +9542,27 @@
       <c r="R4" s="109">
         <v>44</v>
       </c>
-      <c r="S4" s="70">
+      <c r="S4" s="126">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" s="9">
+        <v>10</v>
+      </c>
+      <c r="U4" s="70">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="107">
         <v>1</v>
       </c>
       <c r="B5" s="121">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B5:B27" si="0">D5+F5+H5+J5+L5+N5+P5+R5+T5</f>
         <v>25</v>
       </c>
       <c r="C5" s="124">
-        <f t="shared" si="1"/>
-        <v>6.7142857142857141E-4</v>
+        <f t="shared" ref="C5:C27" si="1">AVERAGE(E5,G5,I5,K5,M5,O5,Q5,S5,U5)/100</f>
+        <v>5.8750000000000002E-4</v>
       </c>
       <c r="D5" s="109">
         <v>15</v>
@@ -9407,21 +9609,27 @@
       <c r="R5" s="109">
         <v>3</v>
       </c>
-      <c r="S5" s="70">
+      <c r="S5" s="126">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="9">
+        <v>0</v>
+      </c>
+      <c r="U5" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="107">
         <v>2</v>
       </c>
       <c r="B6" s="121">
-        <f>D6+F6+H6+J6+L6+N6+P6+R6</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C6" s="124">
-        <f>AVERAGE(E6,G6,I6,K6,M6,O6,Q6,S6)/100</f>
-        <v>3.7142857142857143E-4</v>
+        <f t="shared" si="1"/>
+        <v>3.2499999999999999E-4</v>
       </c>
       <c r="D6" s="109">
         <v>1</v>
@@ -9468,21 +9676,27 @@
       <c r="R6" s="109">
         <v>4</v>
       </c>
-      <c r="S6" s="70">
+      <c r="S6" s="126">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6" s="9">
+        <v>0</v>
+      </c>
+      <c r="U6" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="107">
         <v>3</v>
       </c>
       <c r="B7" s="121">
-        <f t="shared" ref="B7:B27" si="2">D7+F7+H7+J7+L7+N7+P7+R7</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C7" s="124">
-        <f t="shared" ref="C7:C27" si="3">AVERAGE(E7,G7,I7,K7,M7,O7,Q7,S7)/100</f>
-        <v>5.4285714285714289E-4</v>
+        <f t="shared" si="1"/>
+        <v>4.75E-4</v>
       </c>
       <c r="D7" s="109">
         <v>0</v>
@@ -9529,20 +9743,26 @@
       <c r="R7" s="109">
         <v>2</v>
       </c>
-      <c r="S7" s="70">
+      <c r="S7" s="126">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7" s="9">
+        <v>0</v>
+      </c>
+      <c r="U7" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="107">
         <v>4</v>
       </c>
       <c r="B8" s="121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C8" s="124">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D8" s="109">
@@ -9590,20 +9810,26 @@
       <c r="R8" s="109">
         <v>0</v>
       </c>
-      <c r="S8" s="70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" s="116" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S8" s="126">
+        <v>0</v>
+      </c>
+      <c r="T8" s="9">
+        <v>0</v>
+      </c>
+      <c r="U8" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="116" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="113">
         <v>5</v>
       </c>
       <c r="B9" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C9" s="125">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D9" s="115">
@@ -9651,21 +9877,27 @@
       <c r="R9" s="115">
         <v>0</v>
       </c>
-      <c r="S9" s="129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S9" s="127">
+        <v>0</v>
+      </c>
+      <c r="T9" s="114">
+        <v>0</v>
+      </c>
+      <c r="U9" s="129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="107">
         <v>6</v>
       </c>
       <c r="B10" s="121">
-        <f t="shared" si="2"/>
-        <v>1130</v>
+        <f t="shared" si="0"/>
+        <v>1188</v>
       </c>
       <c r="C10" s="124">
-        <f t="shared" si="3"/>
-        <v>3.161428571428572E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.5087500000000008E-2</v>
       </c>
       <c r="D10" s="109">
         <v>199</v>
@@ -9712,21 +9944,27 @@
       <c r="R10" s="109">
         <v>126</v>
       </c>
-      <c r="S10" s="70">
+      <c r="S10" s="126">
         <v>2.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10" s="9">
+        <v>58</v>
+      </c>
+      <c r="U10" s="70">
+        <v>5.94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="107">
         <v>7</v>
       </c>
       <c r="B11" s="121">
-        <f t="shared" si="2"/>
-        <v>42</v>
+        <f t="shared" si="0"/>
+        <v>44</v>
       </c>
       <c r="C11" s="124">
-        <f t="shared" si="3"/>
-        <v>9.4285714285714296E-4</v>
+        <f t="shared" si="1"/>
+        <v>1.0750000000000002E-3</v>
       </c>
       <c r="D11" s="109">
         <v>4</v>
@@ -9773,21 +10011,27 @@
       <c r="R11" s="109">
         <v>3</v>
       </c>
-      <c r="S11" s="70">
+      <c r="S11" s="126">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11" s="9">
+        <v>2</v>
+      </c>
+      <c r="U11" s="70">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="107">
         <v>8</v>
       </c>
       <c r="B12" s="121">
-        <f t="shared" si="2"/>
-        <v>198</v>
+        <f t="shared" si="0"/>
+        <v>206</v>
       </c>
       <c r="C12" s="124">
-        <f t="shared" si="3"/>
-        <v>6.1999999999999998E-3</v>
+        <f t="shared" si="1"/>
+        <v>6.45E-3</v>
       </c>
       <c r="D12" s="109">
         <v>28</v>
@@ -9834,21 +10078,27 @@
       <c r="R12" s="109">
         <v>21</v>
       </c>
-      <c r="S12" s="70">
+      <c r="S12" s="126">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12" s="9">
+        <v>8</v>
+      </c>
+      <c r="U12" s="70">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="107">
         <v>9</v>
       </c>
       <c r="B13" s="121">
-        <f t="shared" si="2"/>
-        <v>58</v>
+        <f t="shared" si="0"/>
+        <v>64</v>
       </c>
       <c r="C13" s="124">
-        <f t="shared" si="3"/>
-        <v>1.5571428571428572E-3</v>
+        <f t="shared" si="1"/>
+        <v>2.1250000000000002E-3</v>
       </c>
       <c r="D13" s="109">
         <v>8</v>
@@ -9895,21 +10145,27 @@
       <c r="R13" s="109">
         <v>8</v>
       </c>
-      <c r="S13" s="70">
+      <c r="S13" s="126">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13" s="9">
+        <v>6</v>
+      </c>
+      <c r="U13" s="70">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="107">
         <v>10</v>
       </c>
       <c r="B14" s="121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C14" s="124">
-        <f t="shared" si="3"/>
-        <v>5.7142857142857142E-5</v>
+        <f t="shared" si="1"/>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="D14" s="109">
         <v>0</v>
@@ -9956,21 +10212,27 @@
       <c r="R14" s="109">
         <v>1</v>
       </c>
-      <c r="S14" s="70">
+      <c r="S14" s="126">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14" s="9">
+        <v>0</v>
+      </c>
+      <c r="U14" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="107">
         <v>11</v>
       </c>
       <c r="B15" s="121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C15" s="124">
-        <f t="shared" si="3"/>
-        <v>1.4285714285714287E-4</v>
+        <f t="shared" si="1"/>
+        <v>1.25E-4</v>
       </c>
       <c r="D15" s="109">
         <v>0</v>
@@ -10017,20 +10279,26 @@
       <c r="R15" s="109">
         <v>0</v>
       </c>
-      <c r="S15" s="70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" s="116" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S15" s="126">
+        <v>0</v>
+      </c>
+      <c r="T15" s="9">
+        <v>0</v>
+      </c>
+      <c r="U15" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="116" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="113">
         <v>12</v>
       </c>
       <c r="B16" s="123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C16" s="125">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D16" s="115">
@@ -10078,21 +10346,27 @@
       <c r="R16" s="115">
         <v>0</v>
       </c>
-      <c r="S16" s="129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S16" s="127">
+        <v>0</v>
+      </c>
+      <c r="T16" s="114">
+        <v>0</v>
+      </c>
+      <c r="U16" s="129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="107">
         <v>13</v>
       </c>
       <c r="B17" s="121">
-        <f t="shared" si="2"/>
-        <v>73</v>
+        <f t="shared" si="0"/>
+        <v>74</v>
       </c>
       <c r="C17" s="124">
-        <f t="shared" si="3"/>
-        <v>2.0285714285714286E-3</v>
+        <f t="shared" si="1"/>
+        <v>1.9E-3</v>
       </c>
       <c r="D17" s="109">
         <v>18</v>
@@ -10139,21 +10413,27 @@
       <c r="R17" s="109">
         <v>6</v>
       </c>
-      <c r="S17" s="70">
+      <c r="S17" s="126">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17" s="9">
+        <v>1</v>
+      </c>
+      <c r="U17" s="70">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="107">
         <v>14</v>
       </c>
       <c r="B18" s="121">
-        <f t="shared" si="2"/>
-        <v>208</v>
+        <f t="shared" si="0"/>
+        <v>209</v>
       </c>
       <c r="C18" s="124">
-        <f t="shared" si="3"/>
-        <v>5.1142857142857136E-3</v>
+        <f t="shared" si="1"/>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="D18" s="109">
         <v>34</v>
@@ -10200,21 +10480,27 @@
       <c r="R18" s="109">
         <v>27</v>
       </c>
-      <c r="S18" s="70">
+      <c r="S18" s="126">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18" s="9">
+        <v>1</v>
+      </c>
+      <c r="U18" s="70">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="107">
         <v>15</v>
       </c>
       <c r="B19" s="121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>133</v>
       </c>
       <c r="C19" s="124">
-        <f t="shared" si="3"/>
-        <v>3.3E-3</v>
+        <f t="shared" si="1"/>
+        <v>2.8874999999999999E-3</v>
       </c>
       <c r="D19" s="109">
         <v>27</v>
@@ -10261,21 +10547,27 @@
       <c r="R19" s="109">
         <v>33</v>
       </c>
-      <c r="S19" s="70">
+      <c r="S19" s="126">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="9">
+        <v>0</v>
+      </c>
+      <c r="U19" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="107">
         <v>16</v>
       </c>
       <c r="B20" s="121">
-        <f t="shared" si="2"/>
-        <v>128</v>
+        <f t="shared" si="0"/>
+        <v>130</v>
       </c>
       <c r="C20" s="124">
-        <f t="shared" si="3"/>
-        <v>3.1571428571428571E-3</v>
+        <f t="shared" si="1"/>
+        <v>3.0125E-3</v>
       </c>
       <c r="D20" s="109">
         <v>17</v>
@@ -10322,21 +10614,27 @@
       <c r="R20" s="109">
         <v>13</v>
       </c>
-      <c r="S20" s="70">
+      <c r="S20" s="126">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20" s="9">
+        <v>2</v>
+      </c>
+      <c r="U20" s="70">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="107">
         <v>17</v>
       </c>
       <c r="B21" s="121">
-        <f t="shared" si="2"/>
-        <v>247</v>
+        <f t="shared" si="0"/>
+        <v>253</v>
       </c>
       <c r="C21" s="124">
-        <f t="shared" si="3"/>
-        <v>5.8142857142857128E-3</v>
+        <f t="shared" si="1"/>
+        <v>5.8499999999999993E-3</v>
       </c>
       <c r="D21" s="109">
         <v>17</v>
@@ -10383,21 +10681,27 @@
       <c r="R21" s="109">
         <v>30</v>
       </c>
-      <c r="S21" s="70">
+      <c r="S21" s="126">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T21" s="9">
+        <v>6</v>
+      </c>
+      <c r="U21" s="70">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="107">
         <v>18</v>
       </c>
       <c r="B22" s="121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C22" s="124">
-        <f t="shared" si="3"/>
-        <v>5.285714285714287E-4</v>
+        <f t="shared" si="1"/>
+        <v>4.6250000000000007E-4</v>
       </c>
       <c r="D22" s="109">
         <v>7</v>
@@ -10444,21 +10748,27 @@
       <c r="R22" s="109">
         <v>1</v>
       </c>
-      <c r="S22" s="70">
+      <c r="S22" s="126">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T22" s="9">
+        <v>0</v>
+      </c>
+      <c r="U22" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="107">
         <v>19</v>
       </c>
       <c r="B23" s="121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C23" s="124">
-        <f t="shared" si="3"/>
-        <v>8.5714285714285713E-5</v>
+        <f t="shared" si="1"/>
+        <v>7.4999999999999993E-5</v>
       </c>
       <c r="D23" s="109">
         <v>1</v>
@@ -10505,21 +10815,27 @@
       <c r="R23" s="109">
         <v>1</v>
       </c>
-      <c r="S23" s="70">
+      <c r="S23" s="126">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T23" s="9">
+        <v>0</v>
+      </c>
+      <c r="U23" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="107">
         <v>20</v>
       </c>
       <c r="B24" s="121">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="C24" s="124">
-        <f t="shared" si="3"/>
-        <v>5.4285714285714289E-4</v>
+        <f t="shared" si="1"/>
+        <v>6.0000000000000016E-4</v>
       </c>
       <c r="D24" s="109">
         <v>1</v>
@@ -10566,21 +10882,27 @@
       <c r="R24" s="109">
         <v>2</v>
       </c>
-      <c r="S24" s="70">
+      <c r="S24" s="126">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" s="116" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T24" s="9">
+        <v>1</v>
+      </c>
+      <c r="U24" s="70">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" s="116" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="113">
         <v>21</v>
       </c>
       <c r="B25" s="123">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="C25" s="125">
-        <f t="shared" si="3"/>
-        <v>1.5714285714285716E-4</v>
+        <f t="shared" si="1"/>
+        <v>2.6250000000000004E-4</v>
       </c>
       <c r="D25" s="115">
         <v>2</v>
@@ -10627,21 +10949,27 @@
       <c r="R25" s="115">
         <v>0</v>
       </c>
-      <c r="S25" s="129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" s="141" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S25" s="127">
+        <v>0</v>
+      </c>
+      <c r="T25" s="114">
+        <v>1</v>
+      </c>
+      <c r="U25" s="129">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" s="141" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="149">
         <v>22</v>
       </c>
       <c r="B26" s="135">
-        <f t="shared" si="2"/>
-        <v>608</v>
+        <f t="shared" si="0"/>
+        <v>626</v>
       </c>
       <c r="C26" s="136">
-        <f t="shared" si="3"/>
-        <v>1.5671428571428572E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.6012499999999999E-2</v>
       </c>
       <c r="D26" s="137">
         <v>84</v>
@@ -10688,23 +11016,29 @@
       <c r="R26" s="137">
         <v>76</v>
       </c>
-      <c r="S26" s="140">
+      <c r="S26" s="138">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" s="141" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="113">
+      <c r="T26" s="139">
+        <v>18</v>
+      </c>
+      <c r="U26" s="140">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" s="141" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="149">
         <v>23</v>
       </c>
-      <c r="B27" s="123">
-        <f t="shared" si="2"/>
-        <v>33893</v>
-      </c>
-      <c r="C27" s="125">
-        <f t="shared" si="3"/>
-        <v>0.91504285714285727</v>
-      </c>
-      <c r="D27" s="115">
+      <c r="B27" s="135">
+        <f t="shared" si="0"/>
+        <v>34755</v>
+      </c>
+      <c r="C27" s="136">
+        <f t="shared" si="1"/>
+        <v>0.91106250000000022</v>
+      </c>
+      <c r="D27" s="137">
         <v>4373</v>
       </c>
       <c r="E27" s="138">
@@ -10749,15 +11083,21 @@
       <c r="R27" s="137">
         <v>5211</v>
       </c>
-      <c r="S27" s="140">
+      <c r="S27" s="138">
         <v>92.85</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T27" s="139">
+        <v>862</v>
+      </c>
+      <c r="U27" s="140">
+        <v>88.32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B28" s="121"/>
-      <c r="C28" s="171">
+      <c r="C28" s="155">
         <f>SUM(C4:C27)</f>
-        <v>0.99991428571428587</v>
+        <v>0.99987500000000029</v>
       </c>
       <c r="E28" s="126"/>
       <c r="G28" s="126"/>
@@ -10766,9 +11106,11 @@
       <c r="M28" s="126"/>
       <c r="O28" s="128"/>
       <c r="Q28" s="128"/>
-      <c r="S28" s="70"/>
-    </row>
-    <row r="29" spans="1:19" s="116" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S28" s="126"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="70"/>
+    </row>
+    <row r="29" spans="1:21" s="116" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="113" t="s">
         <v>288</v>
       </c>
@@ -10819,21 +11161,27 @@
       <c r="R29" s="115" t="s">
         <v>286</v>
       </c>
-      <c r="S29" s="129" t="s">
+      <c r="S29" s="127" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" s="141" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T29" s="114" t="s">
+        <v>286</v>
+      </c>
+      <c r="U29" s="129" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" s="141" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="134">
         <v>1</v>
       </c>
       <c r="B30" s="135">
-        <f>D30+F30+H30+J30+L30+N30+P30+R30</f>
-        <v>33893</v>
+        <f>D30+F30+H30+J30+L30+N30+P30+R30+T30</f>
+        <v>34755</v>
       </c>
       <c r="C30" s="136">
-        <f>AVERAGE(E30,G30,I30,K30,M30,O30,Q30,S30)/100</f>
-        <v>0.91504285714285727</v>
+        <f>AVERAGE(E30,G30,I30,K30,M30,O30,Q30,S30,U30)/100</f>
+        <v>0.91106250000000022</v>
       </c>
       <c r="D30" s="137">
         <v>4373</v>
@@ -10880,21 +11228,27 @@
       <c r="R30" s="137">
         <v>5211</v>
       </c>
-      <c r="S30" s="140">
+      <c r="S30" s="138">
         <v>92.85</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" s="116" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T30" s="139">
+        <v>862</v>
+      </c>
+      <c r="U30" s="140">
+        <v>88.32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" s="116" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="133">
         <v>2</v>
       </c>
       <c r="B31" s="135">
-        <f t="shared" ref="B31:B34" si="4">D31+F31+H31+J31+L31+N31+P31+R31</f>
-        <v>608</v>
+        <f t="shared" ref="B31:B34" si="2">D31+F31+H31+J31+L31+N31+P31+R31+T31</f>
+        <v>626</v>
       </c>
       <c r="C31" s="136">
-        <f t="shared" ref="C31:C34" si="5">AVERAGE(E31,G31,I31,K31,M31,O31,Q31,S31)/100</f>
-        <v>1.5671428571428572E-2</v>
+        <f t="shared" ref="C31:C34" si="3">AVERAGE(E31,G31,I31,K31,M31,O31,Q31,S31,U31)/100</f>
+        <v>1.6012499999999999E-2</v>
       </c>
       <c r="D31" s="115">
         <v>84</v>
@@ -10941,21 +11295,27 @@
       <c r="R31" s="115">
         <v>76</v>
       </c>
-      <c r="S31" s="129">
+      <c r="S31" s="127">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" s="116" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T31" s="114">
+        <v>18</v>
+      </c>
+      <c r="U31" s="129">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" s="116" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="132">
         <v>3</v>
       </c>
       <c r="B32" s="135">
-        <f t="shared" si="4"/>
-        <v>834</v>
+        <f t="shared" si="2"/>
+        <v>846</v>
       </c>
       <c r="C32" s="136">
-        <f t="shared" si="5"/>
-        <v>2.0742857142857143E-2</v>
+        <f t="shared" si="3"/>
+        <v>1.96875E-2</v>
       </c>
       <c r="D32" s="115">
         <v>124</v>
@@ -11002,21 +11362,27 @@
       <c r="R32" s="115">
         <v>113</v>
       </c>
-      <c r="S32" s="129">
+      <c r="S32" s="127">
         <v>2.0099999999999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" s="116" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T32" s="114">
+        <v>12</v>
+      </c>
+      <c r="U32" s="129">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" s="116" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="131">
         <v>4</v>
       </c>
       <c r="B33" s="135">
-        <f t="shared" si="4"/>
-        <v>1438</v>
+        <f t="shared" si="2"/>
+        <v>1512</v>
       </c>
       <c r="C33" s="136">
-        <f t="shared" si="5"/>
-        <v>4.0557142857142861E-2</v>
+        <f t="shared" si="3"/>
+        <v>4.4962499999999996E-2</v>
       </c>
       <c r="D33" s="115">
         <v>239</v>
@@ -11063,21 +11429,27 @@
       <c r="R33" s="115">
         <v>159</v>
       </c>
-      <c r="S33" s="129">
+      <c r="S33" s="127">
         <v>2.83</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" s="116" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T33" s="114">
+        <v>74</v>
+      </c>
+      <c r="U33" s="129">
+        <v>7.58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" s="116" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="130">
         <v>5</v>
       </c>
       <c r="B34" s="135">
-        <f t="shared" si="4"/>
-        <v>315</v>
+        <f t="shared" si="2"/>
+        <v>325</v>
       </c>
       <c r="C34" s="136">
-        <f t="shared" si="5"/>
-        <v>7.9428571428571439E-3</v>
+        <f t="shared" si="3"/>
+        <v>8.2249999999999997E-3</v>
       </c>
       <c r="D34" s="115">
         <v>60</v>
@@ -11124,63 +11496,69 @@
       <c r="R34" s="115">
         <v>53</v>
       </c>
-      <c r="S34" s="129">
+      <c r="S34" s="127">
         <v>0.94</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T34" s="114">
+        <v>10</v>
+      </c>
+      <c r="U34" s="129">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B35" s="121"/>
       <c r="C35" s="122"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B36" s="121"/>
       <c r="C36" s="122"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B37" s="121"/>
       <c r="C37" s="122"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B38" s="121"/>
       <c r="C38" s="122"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B39" s="121"/>
       <c r="C39" s="122"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B40" s="121"/>
       <c r="C40" s="122"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B41" s="121"/>
       <c r="C41" s="122"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B42" s="121"/>
       <c r="C42" s="122"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" s="121"/>
       <c r="C43" s="122"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B44" s="121"/>
       <c r="C44" s="122"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B45" s="121"/>
       <c r="C45" s="122"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B46" s="121"/>
       <c r="C46" s="122"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B47" s="121"/>
       <c r="C47" s="122"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B48" s="121"/>
       <c r="C48" s="122"/>
     </row>
@@ -11335,10 +11713,10 @@
       <c r="A3" s="108" t="s">
         <v>285</v>
       </c>
-      <c r="B3" s="165" t="s">
+      <c r="B3" s="168" t="s">
         <v>291</v>
       </c>
-      <c r="C3" s="166"/>
+      <c r="C3" s="169"/>
       <c r="D3" s="110"/>
       <c r="E3" s="106"/>
       <c r="F3" s="104"/>

</xml_diff>